<commit_message>
Created Save History, Fixed graph x ticks
</commit_message>
<xml_diff>
--- a/Testing/Settings/Budget Simulation - Admin.xlsx
+++ b/Testing/Settings/Budget Simulation - Admin.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Documents\GitHub\Budget-Simulation-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Documents\GitHub\Budget-Simulation-Project\Testing\Settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7648540-999E-478C-93E0-9AFA86AC64A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8DBE589-7D16-4BC3-9EE9-170B8B98AEED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4749EA82-5507-43F6-8DEA-C3E93E89C445}"/>
   </bookViews>
@@ -69,14 +69,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>Deployment #</t>
   </si>
   <si>
-    <t>Highland Price**</t>
-  </si>
-  <si>
     <t>Year</t>
   </si>
   <si>
@@ -114,6 +111,24 @@
   </si>
   <si>
     <t>Highland Contract</t>
+  </si>
+  <si>
+    <t>Highland Price $</t>
+  </si>
+  <si>
+    <t>Deployment Year Lower Bound</t>
+  </si>
+  <si>
+    <t>Contract Term Upper Bound</t>
+  </si>
+  <si>
+    <t>(≤)</t>
+  </si>
+  <si>
+    <t>(≥)</t>
+  </si>
+  <si>
+    <t>Contract Term Lower Bound</t>
   </si>
 </sst>
 </file>
@@ -125,7 +140,7 @@
     <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0_);_([$$-409]* \(#,##0\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -194,6 +209,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF202124"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -324,7 +345,7 @@
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -346,7 +367,6 @@
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -365,10 +385,14 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -688,7 +712,7 @@
   <dimension ref="C3:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -696,7 +720,7 @@
     <col min="1" max="2" width="3.33203125" customWidth="1"/>
     <col min="3" max="3" width="34.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.77734375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19.21875" bestFit="1" customWidth="1"/>
@@ -704,52 +728,52 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:11" ht="21" x14ac:dyDescent="0.4">
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24" t="s">
+      <c r="H3" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+    </row>
+    <row r="4" spans="3:11" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C4" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="15">
+        <v>100000</v>
+      </c>
+      <c r="H4" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="J4" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="17"/>
+    </row>
+    <row r="5" spans="3:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="C5" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="24" t="s">
         <v>4</v>
-      </c>
-      <c r="H3" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-    </row>
-    <row r="4" spans="3:11" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C4" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="15">
-        <v>30000</v>
-      </c>
-      <c r="H4" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="I4" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="J4" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="K4" s="18"/>
-    </row>
-    <row r="5" spans="3:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="C5" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="25" t="s">
-        <v>5</v>
       </c>
       <c r="E5" s="16">
         <v>0.03</v>
       </c>
-      <c r="H5" s="19">
+      <c r="H5" s="18">
         <v>1</v>
       </c>
       <c r="I5" s="9">
@@ -758,19 +782,19 @@
       <c r="J5" s="10">
         <v>22000</v>
       </c>
-      <c r="K5" s="18"/>
+      <c r="K5" s="17"/>
     </row>
     <row r="6" spans="3:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="C6" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>5</v>
+      <c r="C6" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>4</v>
       </c>
       <c r="E6" s="16">
         <v>0.05</v>
       </c>
-      <c r="H6" s="19">
+      <c r="H6" s="18">
         <v>2</v>
       </c>
       <c r="I6" s="11">
@@ -780,19 +804,19 @@
         <f>J5</f>
         <v>22000</v>
       </c>
-      <c r="K6" s="18"/>
+      <c r="K6" s="17"/>
     </row>
     <row r="7" spans="3:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="C7" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="25" t="s">
-        <v>5</v>
+      <c r="C7" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>4</v>
       </c>
       <c r="E7" s="16">
         <v>0.15</v>
       </c>
-      <c r="H7" s="19">
+      <c r="H7" s="18">
         <v>3</v>
       </c>
       <c r="I7" s="11">
@@ -802,19 +826,19 @@
         <f>J6</f>
         <v>22000</v>
       </c>
-      <c r="K7" s="22"/>
+      <c r="K7" s="21"/>
     </row>
     <row r="8" spans="3:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="C8" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="25" t="s">
-        <v>5</v>
+      <c r="C8" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>4</v>
       </c>
       <c r="E8" s="16">
         <v>0.02</v>
       </c>
-      <c r="H8" s="19">
+      <c r="H8" s="18">
         <v>4</v>
       </c>
       <c r="I8" s="13">
@@ -824,19 +848,19 @@
         <f>J7</f>
         <v>22000</v>
       </c>
-      <c r="K8" s="22"/>
+      <c r="K8" s="21"/>
     </row>
     <row r="9" spans="3:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="C9" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="25" t="s">
-        <v>5</v>
+      <c r="C9" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>4</v>
       </c>
       <c r="E9" s="16">
         <v>0.06</v>
       </c>
-      <c r="H9" s="19">
+      <c r="H9" s="18">
         <v>5</v>
       </c>
       <c r="I9" s="1">
@@ -845,19 +869,19 @@
       <c r="J9" s="2">
         <v>27000</v>
       </c>
-      <c r="K9" s="22"/>
+      <c r="K9" s="21"/>
     </row>
     <row r="10" spans="3:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="C10" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="25" t="s">
-        <v>5</v>
+      <c r="C10" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>4</v>
       </c>
       <c r="E10" s="16">
         <v>0.08</v>
       </c>
-      <c r="H10" s="19">
+      <c r="H10" s="18">
         <v>6</v>
       </c>
       <c r="I10" s="3">
@@ -868,13 +892,19 @@
         <f>J9</f>
         <v>27000</v>
       </c>
-      <c r="K10" s="22"/>
+      <c r="K10" s="21"/>
     </row>
     <row r="11" spans="3:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="H11" s="19">
+      <c r="C11" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="8">
+        <v>2022</v>
+      </c>
+      <c r="H11" s="18">
         <v>7</v>
       </c>
       <c r="I11" s="3">
@@ -885,13 +915,19 @@
         <f>J10</f>
         <v>27000</v>
       </c>
-      <c r="K11" s="22"/>
+      <c r="K11" s="21"/>
     </row>
     <row r="12" spans="3:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="H12" s="19">
+      <c r="C12" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="8">
+        <v>5</v>
+      </c>
+      <c r="H12" s="18">
         <v>8</v>
       </c>
       <c r="I12" s="4">
@@ -902,13 +938,19 @@
         <f>J11</f>
         <v>27000</v>
       </c>
-      <c r="K12" s="22"/>
+      <c r="K12" s="21"/>
     </row>
     <row r="13" spans="3:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="H13" s="19">
+      <c r="C13" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="8">
+        <v>20</v>
+      </c>
+      <c r="H13" s="18">
         <v>9</v>
       </c>
       <c r="I13" s="3">
@@ -918,13 +960,13 @@
       <c r="J13" s="2">
         <v>20000</v>
       </c>
-      <c r="K13" s="22"/>
+      <c r="K13" s="21"/>
     </row>
     <row r="14" spans="3:11" ht="18" x14ac:dyDescent="0.35">
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
-      <c r="H14" s="19">
+      <c r="H14" s="18">
         <v>10</v>
       </c>
       <c r="I14" s="3">
@@ -935,13 +977,13 @@
         <f>J13</f>
         <v>20000</v>
       </c>
-      <c r="K14" s="22"/>
+      <c r="K14" s="21"/>
     </row>
     <row r="15" spans="3:11" ht="18" x14ac:dyDescent="0.35">
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
-      <c r="H15" s="19">
+      <c r="H15" s="18">
         <v>11</v>
       </c>
       <c r="I15" s="3">
@@ -952,13 +994,13 @@
         <f>J14</f>
         <v>20000</v>
       </c>
-      <c r="K15" s="22"/>
+      <c r="K15" s="21"/>
     </row>
     <row r="16" spans="3:11" ht="18" x14ac:dyDescent="0.35">
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
-      <c r="H16" s="19">
+      <c r="H16" s="18">
         <v>12</v>
       </c>
       <c r="I16" s="4">
@@ -969,13 +1011,13 @@
         <f>J15</f>
         <v>20000</v>
       </c>
-      <c r="K16" s="23"/>
+      <c r="K16" s="22"/>
     </row>
     <row r="17" spans="3:11" ht="18" x14ac:dyDescent="0.35">
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
-      <c r="H17" s="19">
+      <c r="H17" s="18">
         <v>13</v>
       </c>
       <c r="I17" s="3">
@@ -985,13 +1027,13 @@
       <c r="J17" s="6">
         <v>24000</v>
       </c>
-      <c r="K17" s="22"/>
+      <c r="K17" s="21"/>
     </row>
     <row r="18" spans="3:11" ht="18" x14ac:dyDescent="0.35">
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
-      <c r="H18" s="19">
+      <c r="H18" s="18">
         <v>14</v>
       </c>
       <c r="I18" s="3">
@@ -1002,13 +1044,13 @@
         <f>J17</f>
         <v>24000</v>
       </c>
-      <c r="K18" s="22"/>
+      <c r="K18" s="21"/>
     </row>
     <row r="19" spans="3:11" ht="18" x14ac:dyDescent="0.35">
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
-      <c r="H19" s="19">
+      <c r="H19" s="18">
         <v>15</v>
       </c>
       <c r="I19" s="3">
@@ -1019,13 +1061,13 @@
         <f>J18</f>
         <v>24000</v>
       </c>
-      <c r="K19" s="22"/>
+      <c r="K19" s="21"/>
     </row>
     <row r="20" spans="3:11" ht="18" x14ac:dyDescent="0.35">
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
-      <c r="H20" s="19">
+      <c r="H20" s="18">
         <v>16</v>
       </c>
       <c r="I20" s="4">
@@ -1036,13 +1078,13 @@
         <f>J19</f>
         <v>24000</v>
       </c>
-      <c r="K20" s="22"/>
+      <c r="K20" s="21"/>
     </row>
     <row r="21" spans="3:11" ht="18" x14ac:dyDescent="0.35">
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
-      <c r="H21" s="19">
+      <c r="H21" s="18">
         <v>17</v>
       </c>
       <c r="I21" s="3">
@@ -1051,13 +1093,13 @@
       <c r="J21" s="2">
         <v>22000</v>
       </c>
-      <c r="K21" s="22"/>
+      <c r="K21" s="21"/>
     </row>
     <row r="22" spans="3:11" ht="18" x14ac:dyDescent="0.35">
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
-      <c r="H22" s="19">
+      <c r="H22" s="18">
         <v>18</v>
       </c>
       <c r="I22" s="3">
@@ -1067,13 +1109,10 @@
         <f>J21</f>
         <v>22000</v>
       </c>
-      <c r="K22" s="22"/>
-    </row>
-    <row r="23" spans="3:11" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="H23" s="19">
+      <c r="K22" s="21"/>
+    </row>
+    <row r="23" spans="3:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H23" s="18">
         <v>19</v>
       </c>
       <c r="I23" s="3">
@@ -1083,26 +1122,26 @@
         <f>J22</f>
         <v>22000</v>
       </c>
-      <c r="K23" s="22"/>
+      <c r="K23" s="21"/>
     </row>
     <row r="24" spans="3:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H24" s="19">
+      <c r="H24" s="18">
         <v>20</v>
       </c>
-      <c r="I24" s="27">
+      <c r="I24" s="25">
         <v>70</v>
       </c>
       <c r="J24" s="7">
         <f>J23</f>
         <v>22000</v>
       </c>
-      <c r="K24" s="21"/>
+      <c r="K24" s="20"/>
     </row>
     <row r="25" spans="3:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H25" s="20"/>
-      <c r="I25" s="21"/>
-      <c r="J25" s="21"/>
-      <c r="K25" s="21"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1115,6 +1154,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A1C30AF05D05F44290B877FBA47E06D7" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c390872fb5ee6617233522a93297a75b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="cf34c0ae-c264-4763-a50e-62e14a974a4b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7125aa1be032bbebc3f6e2a5c96b98de" ns3:_="">
     <xsd:import namespace="cf34c0ae-c264-4763-a50e-62e14a974a4b"/>
@@ -1246,22 +1294,21 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{982C5008-F5A2-4ABF-BFBD-A2038E911280}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F24DADEF-2328-413E-AD3E-4515D429BFEF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1279,7 +1326,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D47DD00B-67E0-413D-95D0-0D029AAB1027}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -1293,12 +1340,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{982C5008-F5A2-4ABF-BFBD-A2038E911280}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Lots of Front end
</commit_message>
<xml_diff>
--- a/Testing/Settings/Budget Simulation - Admin.xlsx
+++ b/Testing/Settings/Budget Simulation - Admin.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Documents\GitHub\Budget-Simulation-Project\Testing\Settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8DBE589-7D16-4BC3-9EE9-170B8B98AEED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F9876F-6301-4DF5-8500-7436FECB8398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4749EA82-5507-43F6-8DEA-C3E93E89C445}"/>
+    <workbookView xWindow="5760" yWindow="2088" windowWidth="17280" windowHeight="8880" xr2:uid="{4749EA82-5507-43F6-8DEA-C3E93E89C445}"/>
   </bookViews>
   <sheets>
     <sheet name="Budget Simulation - Admin" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Deployment #</t>
   </si>
@@ -86,13 +86,7 @@
     <t>(%)</t>
   </si>
   <si>
-    <t>($)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Contract Escalator </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contract Price Bus/Year </t>
   </si>
   <si>
     <t xml:space="preserve">Diesel Price Escalator </t>
@@ -135,10 +129,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0_);_([$$-409]* \(#,##0\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -340,12 +332,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -361,10 +352,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -394,10 +382,9 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="2" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -712,7 +699,7 @@
   <dimension ref="C3:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -728,52 +715,52 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:11" ht="21" x14ac:dyDescent="0.4">
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23" t="s">
+      <c r="D3" s="22"/>
+      <c r="E3" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
+      <c r="H3" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
     </row>
     <row r="4" spans="3:11" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C4" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="24" t="s">
+      <c r="C4" s="23" t="s">
         <v>5</v>
       </c>
+      <c r="D4" s="23" t="s">
+        <v>4</v>
+      </c>
       <c r="E4" s="15">
-        <v>100000</v>
-      </c>
-      <c r="H4" s="26" t="s">
+        <v>0.03</v>
+      </c>
+      <c r="H4" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="26" t="s">
+      <c r="I4" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="J4" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="K4" s="17"/>
+      <c r="J4" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" s="16"/>
     </row>
     <row r="5" spans="3:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="16">
-        <v>0.03</v>
-      </c>
-      <c r="H5" s="18">
+      <c r="E5" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="H5" s="17">
         <v>1</v>
       </c>
       <c r="I5" s="9">
@@ -782,19 +769,19 @@
       <c r="J5" s="10">
         <v>22000</v>
       </c>
-      <c r="K5" s="17"/>
+      <c r="K5" s="16"/>
     </row>
     <row r="6" spans="3:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="16">
-        <v>0.05</v>
-      </c>
-      <c r="H6" s="18">
+      <c r="E6" s="15">
+        <v>0.15</v>
+      </c>
+      <c r="H6" s="17">
         <v>2</v>
       </c>
       <c r="I6" s="11">
@@ -804,19 +791,19 @@
         <f>J5</f>
         <v>22000</v>
       </c>
-      <c r="K6" s="17"/>
+      <c r="K6" s="16"/>
     </row>
     <row r="7" spans="3:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="C7" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="24" t="s">
+      <c r="C7" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="16">
-        <v>0.15</v>
-      </c>
-      <c r="H7" s="18">
+      <c r="E7" s="15">
+        <v>0.02</v>
+      </c>
+      <c r="H7" s="17">
         <v>3</v>
       </c>
       <c r="I7" s="11">
@@ -826,19 +813,19 @@
         <f>J6</f>
         <v>22000</v>
       </c>
-      <c r="K7" s="21"/>
+      <c r="K7" s="20"/>
     </row>
     <row r="8" spans="3:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="16">
-        <v>0.02</v>
-      </c>
-      <c r="H8" s="18">
+      <c r="E8" s="15">
+        <v>0.06</v>
+      </c>
+      <c r="H8" s="17">
         <v>4</v>
       </c>
       <c r="I8" s="13">
@@ -848,19 +835,19 @@
         <f>J7</f>
         <v>22000</v>
       </c>
-      <c r="K8" s="21"/>
+      <c r="K8" s="20"/>
     </row>
     <row r="9" spans="3:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="C9" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="24" t="s">
+      <c r="C9" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="16">
-        <v>0.06</v>
-      </c>
-      <c r="H9" s="18">
+      <c r="E9" s="15">
+        <v>0.08</v>
+      </c>
+      <c r="H9" s="17">
         <v>5</v>
       </c>
       <c r="I9" s="1">
@@ -869,19 +856,10 @@
       <c r="J9" s="2">
         <v>27000</v>
       </c>
-      <c r="K9" s="21"/>
-    </row>
-    <row r="10" spans="3:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="C10" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10" s="16">
-        <v>0.08</v>
-      </c>
-      <c r="H10" s="18">
+      <c r="K9" s="20"/>
+    </row>
+    <row r="10" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="H10" s="17">
         <v>6</v>
       </c>
       <c r="I10" s="3">
@@ -892,19 +870,19 @@
         <f>J9</f>
         <v>27000</v>
       </c>
-      <c r="K10" s="21"/>
+      <c r="K10" s="20"/>
     </row>
     <row r="11" spans="3:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="C11" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="27" t="s">
-        <v>18</v>
+      <c r="C11" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>16</v>
       </c>
       <c r="E11" s="8">
         <v>2022</v>
       </c>
-      <c r="H11" s="18">
+      <c r="H11" s="17">
         <v>7</v>
       </c>
       <c r="I11" s="3">
@@ -915,19 +893,19 @@
         <f>J10</f>
         <v>27000</v>
       </c>
-      <c r="K11" s="21"/>
+      <c r="K11" s="20"/>
     </row>
     <row r="12" spans="3:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="C12" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="27" t="s">
-        <v>18</v>
+      <c r="C12" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>16</v>
       </c>
       <c r="E12" s="8">
         <v>5</v>
       </c>
-      <c r="H12" s="18">
+      <c r="H12" s="17">
         <v>8</v>
       </c>
       <c r="I12" s="4">
@@ -938,19 +916,19 @@
         <f>J11</f>
         <v>27000</v>
       </c>
-      <c r="K12" s="21"/>
+      <c r="K12" s="20"/>
     </row>
     <row r="13" spans="3:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="C13" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="27" t="s">
-        <v>17</v>
+      <c r="C13" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>15</v>
       </c>
       <c r="E13" s="8">
         <v>20</v>
       </c>
-      <c r="H13" s="18">
+      <c r="H13" s="17">
         <v>9</v>
       </c>
       <c r="I13" s="3">
@@ -960,13 +938,13 @@
       <c r="J13" s="2">
         <v>20000</v>
       </c>
-      <c r="K13" s="21"/>
+      <c r="K13" s="20"/>
     </row>
     <row r="14" spans="3:11" ht="18" x14ac:dyDescent="0.35">
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
-      <c r="H14" s="18">
+      <c r="H14" s="17">
         <v>10</v>
       </c>
       <c r="I14" s="3">
@@ -977,13 +955,13 @@
         <f>J13</f>
         <v>20000</v>
       </c>
-      <c r="K14" s="21"/>
+      <c r="K14" s="20"/>
     </row>
     <row r="15" spans="3:11" ht="18" x14ac:dyDescent="0.35">
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
-      <c r="H15" s="18">
+      <c r="H15" s="17">
         <v>11</v>
       </c>
       <c r="I15" s="3">
@@ -994,13 +972,13 @@
         <f>J14</f>
         <v>20000</v>
       </c>
-      <c r="K15" s="21"/>
+      <c r="K15" s="20"/>
     </row>
     <row r="16" spans="3:11" ht="18" x14ac:dyDescent="0.35">
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
-      <c r="H16" s="18">
+      <c r="H16" s="17">
         <v>12</v>
       </c>
       <c r="I16" s="4">
@@ -1011,13 +989,13 @@
         <f>J15</f>
         <v>20000</v>
       </c>
-      <c r="K16" s="22"/>
+      <c r="K16" s="21"/>
     </row>
     <row r="17" spans="3:11" ht="18" x14ac:dyDescent="0.35">
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
-      <c r="H17" s="18">
+      <c r="H17" s="17">
         <v>13</v>
       </c>
       <c r="I17" s="3">
@@ -1027,13 +1005,13 @@
       <c r="J17" s="6">
         <v>24000</v>
       </c>
-      <c r="K17" s="21"/>
+      <c r="K17" s="20"/>
     </row>
     <row r="18" spans="3:11" ht="18" x14ac:dyDescent="0.35">
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
-      <c r="H18" s="18">
+      <c r="H18" s="17">
         <v>14</v>
       </c>
       <c r="I18" s="3">
@@ -1044,13 +1022,13 @@
         <f>J17</f>
         <v>24000</v>
       </c>
-      <c r="K18" s="21"/>
+      <c r="K18" s="20"/>
     </row>
     <row r="19" spans="3:11" ht="18" x14ac:dyDescent="0.35">
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
-      <c r="H19" s="18">
+      <c r="H19" s="17">
         <v>15</v>
       </c>
       <c r="I19" s="3">
@@ -1061,13 +1039,13 @@
         <f>J18</f>
         <v>24000</v>
       </c>
-      <c r="K19" s="21"/>
+      <c r="K19" s="20"/>
     </row>
     <row r="20" spans="3:11" ht="18" x14ac:dyDescent="0.35">
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
-      <c r="H20" s="18">
+      <c r="H20" s="17">
         <v>16</v>
       </c>
       <c r="I20" s="4">
@@ -1078,13 +1056,13 @@
         <f>J19</f>
         <v>24000</v>
       </c>
-      <c r="K20" s="21"/>
+      <c r="K20" s="20"/>
     </row>
     <row r="21" spans="3:11" ht="18" x14ac:dyDescent="0.35">
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
-      <c r="H21" s="18">
+      <c r="H21" s="17">
         <v>17</v>
       </c>
       <c r="I21" s="3">
@@ -1093,13 +1071,10 @@
       <c r="J21" s="2">
         <v>22000</v>
       </c>
-      <c r="K21" s="21"/>
-    </row>
-    <row r="22" spans="3:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="H22" s="18">
+      <c r="K21" s="20"/>
+    </row>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="H22" s="17">
         <v>18</v>
       </c>
       <c r="I22" s="3">
@@ -1109,10 +1084,10 @@
         <f>J21</f>
         <v>22000</v>
       </c>
-      <c r="K22" s="21"/>
+      <c r="K22" s="20"/>
     </row>
     <row r="23" spans="3:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H23" s="18">
+      <c r="H23" s="17">
         <v>19</v>
       </c>
       <c r="I23" s="3">
@@ -1122,26 +1097,26 @@
         <f>J22</f>
         <v>22000</v>
       </c>
-      <c r="K23" s="21"/>
+      <c r="K23" s="20"/>
     </row>
     <row r="24" spans="3:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H24" s="18">
+      <c r="H24" s="17">
         <v>20</v>
       </c>
-      <c r="I24" s="25">
+      <c r="I24" s="24">
         <v>70</v>
       </c>
       <c r="J24" s="7">
         <f>J23</f>
         <v>22000</v>
       </c>
-      <c r="K24" s="20"/>
+      <c r="K24" s="19"/>
     </row>
     <row r="25" spans="3:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H25" s="19"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="20"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1154,12 +1129,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1295,15 +1267,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{982C5008-F5A2-4ABF-BFBD-A2038E911280}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D47DD00B-67E0-413D-95D0-0D029AAB1027}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="cf34c0ae-c264-4763-a50e-62e14a974a4b"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1327,17 +1310,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D47DD00B-67E0-413D-95D0-0D029AAB1027}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{982C5008-F5A2-4ABF-BFBD-A2038E911280}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="cf34c0ae-c264-4763-a50e-62e14a974a4b"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Code rewrite, name your price functions, nyp table, saving/backup features
</commit_message>
<xml_diff>
--- a/Testing/Settings/Budget Simulation - Admin.xlsx
+++ b/Testing/Settings/Budget Simulation - Admin.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Documents\GitHub\Budget-Simulation-Project\Testing\Settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F9876F-6301-4DF5-8500-7436FECB8398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A93CA34A-3D30-443E-B699-F3F8E4826736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="2088" windowWidth="17280" windowHeight="8880" xr2:uid="{4749EA82-5507-43F6-8DEA-C3E93E89C445}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4749EA82-5507-43F6-8DEA-C3E93E89C445}"/>
   </bookViews>
   <sheets>
     <sheet name="Budget Simulation - Admin" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
   <si>
     <t>Deployment #</t>
   </si>
@@ -123,6 +123,15 @@
   </si>
   <si>
     <t>Contract Term Lower Bound</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Budget Simulation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name Your Price </t>
+  </si>
+  <si>
+    <t>Years to Deploy Upper Bound</t>
   </si>
 </sst>
 </file>
@@ -132,7 +141,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0_);_([$$-409]* \(#,##0\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,6 +216,19 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -336,7 +358,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -380,6 +402,12 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -699,7 +727,7 @@
   <dimension ref="C3:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -729,16 +757,12 @@
       <c r="J3" s="27"/>
       <c r="K3" s="27"/>
     </row>
-    <row r="4" spans="3:11" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C4" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="15">
-        <v>0.03</v>
-      </c>
+    <row r="4" spans="3:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C4" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
       <c r="H4" s="25" t="s">
         <v>1</v>
       </c>
@@ -750,15 +774,15 @@
       </c>
       <c r="K4" s="16"/>
     </row>
-    <row r="5" spans="3:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:11" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C5" s="23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5" s="23" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="15">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="H5" s="17">
         <v>1</v>
@@ -773,13 +797,13 @@
     </row>
     <row r="6" spans="3:11" ht="18" x14ac:dyDescent="0.35">
       <c r="C6" s="23" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D6" s="23" t="s">
         <v>4</v>
       </c>
       <c r="E6" s="15">
-        <v>0.15</v>
+        <v>0.05</v>
       </c>
       <c r="H6" s="17">
         <v>2</v>
@@ -795,13 +819,13 @@
     </row>
     <row r="7" spans="3:11" ht="18" x14ac:dyDescent="0.35">
       <c r="C7" s="23" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D7" s="23" t="s">
         <v>4</v>
       </c>
       <c r="E7" s="15">
-        <v>0.02</v>
+        <v>0.15</v>
       </c>
       <c r="H7" s="17">
         <v>3</v>
@@ -817,13 +841,13 @@
     </row>
     <row r="8" spans="3:11" ht="18" x14ac:dyDescent="0.35">
       <c r="C8" s="23" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D8" s="23" t="s">
         <v>4</v>
       </c>
       <c r="E8" s="15">
-        <v>0.06</v>
+        <v>0.02</v>
       </c>
       <c r="H8" s="17">
         <v>4</v>
@@ -839,13 +863,13 @@
     </row>
     <row r="9" spans="3:11" ht="18" x14ac:dyDescent="0.35">
       <c r="C9" s="23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9" s="23" t="s">
         <v>4</v>
       </c>
       <c r="E9" s="15">
-        <v>0.08</v>
+        <v>0.06</v>
       </c>
       <c r="H9" s="17">
         <v>5</v>
@@ -858,7 +882,16 @@
       </c>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="C10" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="15">
+        <v>0.08</v>
+      </c>
       <c r="H10" s="17">
         <v>6</v>
       </c>
@@ -872,16 +905,7 @@
       </c>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="3:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="C11" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="8">
-        <v>2022</v>
-      </c>
+    <row r="11" spans="3:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H11" s="17">
         <v>7</v>
       </c>
@@ -897,13 +921,13 @@
     </row>
     <row r="12" spans="3:11" ht="18" x14ac:dyDescent="0.35">
       <c r="C12" s="23" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D12" s="26" t="s">
         <v>16</v>
       </c>
       <c r="E12" s="8">
-        <v>5</v>
+        <v>2022</v>
       </c>
       <c r="H12" s="17">
         <v>8</v>
@@ -920,13 +944,13 @@
     </row>
     <row r="13" spans="3:11" ht="18" x14ac:dyDescent="0.35">
       <c r="C13" s="23" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E13" s="8">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="H13" s="17">
         <v>9</v>
@@ -941,9 +965,15 @@
       <c r="K13" s="20"/>
     </row>
     <row r="14" spans="3:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
+      <c r="C14" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="8">
+        <v>20</v>
+      </c>
       <c r="H14" s="17">
         <v>10</v>
       </c>
@@ -974,10 +1004,12 @@
       </c>
       <c r="K15" s="20"/>
     </row>
-    <row r="16" spans="3:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
+    <row r="16" spans="3:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="C16" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
       <c r="H16" s="17">
         <v>12</v>
       </c>
@@ -992,9 +1024,15 @@
       <c r="K16" s="21"/>
     </row>
     <row r="17" spans="3:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
+      <c r="C17" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="8">
+        <v>5</v>
+      </c>
       <c r="H17" s="17">
         <v>13</v>
       </c>
@@ -1008,9 +1046,15 @@
       <c r="K17" s="20"/>
     </row>
     <row r="18" spans="3:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
+      <c r="C18" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="8">
+        <v>20</v>
+      </c>
       <c r="H18" s="17">
         <v>14</v>
       </c>
@@ -1025,9 +1069,15 @@
       <c r="K18" s="20"/>
     </row>
     <row r="19" spans="3:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
+      <c r="C19" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="8">
+        <v>20</v>
+      </c>
       <c r="H19" s="17">
         <v>15</v>
       </c>
@@ -1119,8 +1169,10 @@
       <c r="K25" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="H3:K3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C16:E16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -1129,9 +1181,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1267,26 +1322,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D47DD00B-67E0-413D-95D0-0D029AAB1027}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{982C5008-F5A2-4ABF-BFBD-A2038E911280}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="cf34c0ae-c264-4763-a50e-62e14a974a4b"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1310,9 +1354,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{982C5008-F5A2-4ABF-BFBD-A2038E911280}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D47DD00B-67E0-413D-95D0-0D029AAB1027}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="cf34c0ae-c264-4763-a50e-62e14a974a4b"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>